<commit_message>
new changes for assertion and reporting enahancements
</commit_message>
<xml_diff>
--- a/testData/amazonSteps.xlsx
+++ b/testData/amazonSteps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/QATaskAutomation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EFC8614-4894-4D5E-8135-651941460D6D}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8DA181D-4E11-4591-8B65-652D274AB41E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
   <si>
     <t>action</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Search Amazon</t>
   </si>
   <si>
-    <t>Go</t>
-  </si>
-  <si>
     <t>SAMSUNG 85-Inch Class Crystal UHD 4K DU7200 Series HDR Smart TV w/Object Tracking Sound Lite, PurColor, Motion Xcelerator, Mega Contrast, Q-Symphony (UN85DU7200, 2024 Model)</t>
   </si>
   <si>
@@ -166,23 +163,41 @@
     <t>Weaver</t>
   </si>
   <si>
-    <t>#parsersMB2,shipping_amount</t>
-  </si>
-  <si>
-    <t>.</t>
+    <t>https://www.amazon.com</t>
+  </si>
+  <si>
+    <t>keypress</t>
+  </si>
+  <si>
+    <t>Enter</t>
   </si>
   <si>
     <t>no</t>
   </si>
   <si>
-    <t>https://www.amazon.com/SIMPLIHOME-Cocktail-Footrest-Upholstered-Contemporary/dp/B06WV91PNR?th=1</t>
+    <t>cartassert</t>
+  </si>
+  <si>
+    <t>#parsers,items</t>
+  </si>
+  <si>
+    <t>#parsers,discounts</t>
+  </si>
+  <si>
+    <t>#parsers,sales_tax</t>
+  </si>
+  <si>
+    <t>#parsers,shipping_amount</t>
+  </si>
+  <si>
+    <t>#parsers,cart_total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,14 +209,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -228,15 +235,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -520,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,8 +578,8 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="G2" s="1">
         <v>1000</v>
@@ -591,7 +595,7 @@
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -611,14 +615,14 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1">
         <v>1000</v>
@@ -634,11 +638,11 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1">
         <v>1000</v>
@@ -654,17 +658,17 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="1">
         <v>1000</v>
@@ -680,14 +684,14 @@
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1">
         <v>1000</v>
@@ -703,17 +707,17 @@
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1">
         <v>1000</v>
@@ -729,14 +733,14 @@
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1">
         <v>1000</v>
@@ -752,8 +756,8 @@
       <c r="B10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>17</v>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>14</v>
@@ -775,8 +779,8 @@
       <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
@@ -785,7 +789,7 @@
         <v>13</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1">
         <v>1000</v>
@@ -801,14 +805,17 @@
       <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="G12" s="1">
         <v>1000</v>
@@ -824,14 +831,14 @@
       <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>19</v>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -850,14 +857,14 @@
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G14" s="1">
         <v>1000</v>
@@ -877,7 +884,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" s="2"/>
       <c r="G15" s="1">
@@ -895,13 +902,13 @@
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="1">
         <v>1000</v>
@@ -921,10 +928,10 @@
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" s="1">
         <v>1000</v>
@@ -941,13 +948,13 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="G18" s="1">
         <v>1000</v>
@@ -967,10 +974,10 @@
         <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G19" s="1">
         <v>1000</v>
@@ -987,13 +994,13 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" s="1">
         <v>1000</v>
@@ -1013,10 +1020,10 @@
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="G21" s="1">
         <v>1000</v>
@@ -1033,13 +1040,13 @@
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G22" s="1">
         <v>1000</v>
@@ -1056,13 +1063,13 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G23" s="1">
         <v>1000</v>
@@ -1079,16 +1086,96 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G24" s="1">
         <v>1000</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H27" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -1096,10 +1183,11 @@
     <hyperlink ref="F6" r:id="rId1" xr:uid="{7393E911-892C-4F6F-97BB-7A317C41FFB8}"/>
     <hyperlink ref="F8" r:id="rId2" xr:uid="{689D5A8F-41A7-4BB1-961E-DD235DAE98E6}"/>
     <hyperlink ref="D15" r:id="rId3" xr:uid="{B77EF146-4E21-4A86-8EE0-B086C0721682}"/>
-    <hyperlink ref="F24" r:id="rId4" display="weavernormar@gmail.com" xr:uid="{BE8CCFC8-BE97-4DC1-AA5F-DA9F9A55FEA0}"/>
+    <hyperlink ref="F23" r:id="rId4" display="weavernormar@gmail.com" xr:uid="{BE8CCFC8-BE97-4DC1-AA5F-DA9F9A55FEA0}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{25C9805E-CA20-4315-8F78-8F648D8393CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Working code for element finder and assert
</commit_message>
<xml_diff>
--- a/testData/amazonSteps.xlsx
+++ b/testData/amazonSteps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/QATaskAutomation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="371" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8DA181D-4E11-4591-8B65-652D274AB41E}"/>
+  <xr:revisionPtr revIDLastSave="375" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{536B6AD6-DA3D-4718-9F4B-973F61CD1CCD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="54">
   <si>
     <t>action</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>scroll</t>
-  </si>
-  <si>
-    <t>div</t>
   </si>
   <si>
     <t>Continue</t>
@@ -526,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1">
         <v>1000</v>
@@ -601,6 +598,9 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" s="1">
         <v>1000</v>
       </c>
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1">
         <v>1000</v>
@@ -642,7 +642,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="G5" s="1">
         <v>1000</v>
@@ -662,13 +665,13 @@
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1">
         <v>1000</v>
@@ -688,10 +691,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1">
         <v>1000</v>
@@ -711,13 +714,13 @@
         <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1">
         <v>1000</v>
@@ -737,10 +740,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1">
         <v>1000</v>
@@ -754,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>16</v>
@@ -777,7 +780,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -803,10 +806,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>14</v>
@@ -815,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1">
         <v>1000</v>
@@ -829,16 +832,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -855,16 +858,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="G14" s="1">
         <v>1000</v>
@@ -884,7 +887,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="2"/>
       <c r="G15" s="1">
@@ -905,10 +908,10 @@
         <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="1">
         <v>1000</v>
@@ -928,10 +931,10 @@
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="1">
         <v>1000</v>
@@ -951,10 +954,10 @@
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="G18" s="1">
         <v>1000</v>
@@ -974,10 +977,10 @@
         <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="G19" s="1">
         <v>1000</v>
@@ -997,10 +1000,10 @@
         <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="1">
         <v>1000</v>
@@ -1020,10 +1023,10 @@
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G21" s="1">
         <v>1000</v>
@@ -1040,13 +1043,13 @@
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="G22" s="1">
         <v>1000</v>
@@ -1063,13 +1066,13 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="G23" s="1">
         <v>1000</v>
@@ -1086,10 +1089,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="1">
         <v>1000</v>
@@ -1106,10 +1109,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G25" s="1">
         <v>1000</v>
@@ -1126,10 +1129,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G26" s="1">
         <v>1000</v>
@@ -1146,10 +1149,10 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" s="1">
         <v>1000</v>
@@ -1166,10 +1169,10 @@
         <v>11</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="G28" s="1">
         <v>1000</v>

</xml_diff>

<commit_message>
Changes to avoid bot detection and fake retailer
</commit_message>
<xml_diff>
--- a/testData/amazonSteps.xlsx
+++ b/testData/amazonSteps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/QATaskAutomation/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="375" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{536B6AD6-DA3D-4718-9F4B-973F61CD1CCD}"/>
+  <xr:revisionPtr revIDLastSave="376" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CA6F1D4-47F4-4EAA-A0A4-FB481D3B8133}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
   <si>
     <t>action</t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>Enter</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>cartassert</t>
@@ -523,9 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -757,7 +752,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>16</v>
@@ -780,7 +775,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -806,7 +801,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>45</v>
@@ -832,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
@@ -858,7 +853,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
@@ -1089,10 +1084,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G24" s="1">
         <v>1000</v>
@@ -1109,10 +1104,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G25" s="1">
         <v>1000</v>
@@ -1129,10 +1124,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G26" s="1">
         <v>1000</v>
@@ -1149,10 +1144,10 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G27" s="1">
         <v>1000</v>
@@ -1169,10 +1164,10 @@
         <v>11</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="G28" s="1">
         <v>1000</v>

</xml_diff>

<commit_message>
somehow working demo code
</commit_message>
<xml_diff>
--- a/testData/amazonSteps.xlsx
+++ b/testData/amazonSteps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/QATaskAutomation/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/Mytest/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="376" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CA6F1D4-47F4-4EAA-A0A4-FB481D3B8133}"/>
+  <xr:revisionPtr revIDLastSave="382" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DC69E5B-E47F-4181-989B-14FA22419C72}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
   <si>
     <t>action</t>
   </si>
@@ -70,21 +70,12 @@
     <t>input</t>
   </si>
   <si>
-    <t>Search Amazon</t>
-  </si>
-  <si>
-    <t>SAMSUNG 85-Inch Class Crystal UHD 4K DU7200 Series HDR Smart TV w/Object Tracking Sound Lite, PurColor, Motion Xcelerator, Mega Contrast, Q-Symphony (UN85DU7200, 2024 Model)</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>scroll</t>
-  </si>
-  <si>
     <t>Continue</t>
   </si>
   <si>
@@ -106,12 +97,6 @@
     <t>Sign in</t>
   </si>
   <si>
-    <t>Add to cart</t>
-  </si>
-  <si>
-    <t>button</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/gp/cart/view.html?ref_=nav_cart</t>
   </si>
   <si>
@@ -161,12 +146,6 @@
   </si>
   <si>
     <t>https://www.amazon.com</t>
-  </si>
-  <si>
-    <t>keypress</t>
-  </si>
-  <si>
-    <t>Enter</t>
   </si>
   <si>
     <t>cartassert</t>
@@ -518,9 +497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -571,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G2" s="1">
         <v>1000</v>
@@ -594,7 +575,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1">
         <v>1000</v>
@@ -611,13 +592,13 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1">
         <v>1000</v>
@@ -637,10 +618,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="G5" s="1">
         <v>1000</v>
@@ -657,16 +638,16 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G6" s="1">
         <v>1000</v>
@@ -683,13 +664,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G7" s="1">
         <v>1000</v>
@@ -706,16 +687,16 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1">
         <v>1000</v>
@@ -732,13 +713,13 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G9" s="1">
         <v>1000</v>
@@ -755,19 +736,17 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="2"/>
       <c r="G10" s="1">
         <v>1000</v>
       </c>
       <c r="H10" s="1">
-        <v>2000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -778,22 +757,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G11" s="1">
         <v>1000</v>
       </c>
       <c r="H11" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -804,16 +780,13 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="G12" s="1">
         <v>1000</v>
@@ -830,16 +803,13 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1">
         <v>1000</v>
@@ -856,13 +826,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G14" s="1">
         <v>1000</v>
@@ -879,12 +849,14 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G15" s="1">
         <v>1000</v>
       </c>
@@ -900,19 +872,19 @@
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G16" s="1">
         <v>1000</v>
       </c>
       <c r="H16" s="1">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -923,13 +895,13 @@
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G17" s="1">
         <v>1000</v>
@@ -946,13 +918,13 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G18" s="1">
         <v>1000</v>
@@ -969,13 +941,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G19" s="1">
         <v>1000</v>
@@ -992,19 +961,16 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G20" s="1">
         <v>1000</v>
       </c>
       <c r="H20" s="1">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1015,13 +981,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G21" s="1">
         <v>1000</v>
@@ -1038,13 +1001,10 @@
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G22" s="1">
         <v>1000</v>
@@ -1061,118 +1021,15 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G23" s="1">
         <v>1000</v>
       </c>
       <c r="H23" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H24" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H25" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H26" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H27" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G28" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H28" s="1">
         <v>2000</v>
       </c>
     </row>
@@ -1180,8 +1037,8 @@
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{7393E911-892C-4F6F-97BB-7A317C41FFB8}"/>
     <hyperlink ref="F8" r:id="rId2" xr:uid="{689D5A8F-41A7-4BB1-961E-DD235DAE98E6}"/>
-    <hyperlink ref="D15" r:id="rId3" xr:uid="{B77EF146-4E21-4A86-8EE0-B086C0721682}"/>
-    <hyperlink ref="F23" r:id="rId4" display="weavernormar@gmail.com" xr:uid="{BE8CCFC8-BE97-4DC1-AA5F-DA9F9A55FEA0}"/>
+    <hyperlink ref="D10" r:id="rId3" xr:uid="{B77EF146-4E21-4A86-8EE0-B086C0721682}"/>
+    <hyperlink ref="F18" r:id="rId4" display="weavernormar@gmail.com" xr:uid="{BE8CCFC8-BE97-4DC1-AA5F-DA9F9A55FEA0}"/>
     <hyperlink ref="D2" r:id="rId5" xr:uid="{25C9805E-CA20-4315-8F78-8F648D8393CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>